<commit_message>
Better test Excel file
</commit_message>
<xml_diff>
--- a/cmd/xconv/test.xlsx
+++ b/cmd/xconv/test.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15990" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet0" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="153">
   <si>
     <t>Preamble</t>
   </si>
@@ -193,16 +189,305 @@
   </si>
   <si>
     <t>HHH7</t>
+  </si>
+  <si>
+    <t>8/9/2015 9:15 PM</t>
+  </si>
+  <si>
+    <t>9/10/2015 11:15 PM</t>
+  </si>
+  <si>
+    <t>12/1/2015 11:15 AM</t>
+  </si>
+  <si>
+    <t>11/22/2015 9:09 AM</t>
+  </si>
+  <si>
+    <t>12/1/2015 11:15 PM</t>
+  </si>
+  <si>
+    <t>11/22/2015 9:09 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Dealerweb Confidential</t>
+  </si>
+  <si>
+    <t>Entitled User List</t>
+  </si>
+  <si>
+    <t>Barclays Capital</t>
+  </si>
+  <si>
+    <t>Oct 5, 2015 - Oct 9, 2015</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>Logon ID</t>
+  </si>
+  <si>
+    <t>Company Acronym</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Entitlement</t>
+  </si>
+  <si>
+    <t>Authorized?</t>
+  </si>
+  <si>
+    <t>Enabled?</t>
+  </si>
+  <si>
+    <t>View Prices?</t>
+  </si>
+  <si>
+    <t>Trade?</t>
+  </si>
+  <si>
+    <t>Master Blotter?</t>
+  </si>
+  <si>
+    <t>Limit Update?</t>
+  </si>
+  <si>
+    <t>Profile Description</t>
+  </si>
+  <si>
+    <t>Last Logon Date</t>
+  </si>
+  <si>
+    <t>Arnab Nandi</t>
+  </si>
+  <si>
+    <t>anandi</t>
+  </si>
+  <si>
+    <t>BARCAP</t>
+  </si>
+  <si>
+    <t>Arnab</t>
+  </si>
+  <si>
+    <t>Nandi</t>
+  </si>
+  <si>
+    <t>a@a.com</t>
+  </si>
+  <si>
+    <t>EFP</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>DEALER</t>
+  </si>
+  <si>
+    <t>anandi2</t>
+  </si>
+  <si>
+    <t>nandiarnbcdf</t>
+  </si>
+  <si>
+    <t>nandiarnbci</t>
+  </si>
+  <si>
+    <t>B G</t>
+  </si>
+  <si>
+    <t>bgalgano12</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>1@dealerweb.com</t>
+  </si>
+  <si>
+    <t>Cynthia Chuang</t>
+  </si>
+  <si>
+    <t>cchuang</t>
+  </si>
+  <si>
+    <t>Cynthia</t>
+  </si>
+  <si>
+    <t>Chuang</t>
+  </si>
+  <si>
+    <t>cynthia.chuang@barclays.com</t>
+  </si>
+  <si>
+    <t>d s</t>
+  </si>
+  <si>
+    <t>dschmitt98</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>1@1.com</t>
+  </si>
+  <si>
+    <t>Daniel Schmitt</t>
+  </si>
+  <si>
+    <t>dschmitt13</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Schmitt</t>
+  </si>
+  <si>
+    <t>Dara Miller</t>
+  </si>
+  <si>
+    <t>dmiller3</t>
+  </si>
+  <si>
+    <t>Dara</t>
+  </si>
+  <si>
+    <t>Miller</t>
+  </si>
+  <si>
+    <t>Erik Wrolstad</t>
+  </si>
+  <si>
+    <t>ewrolstad</t>
+  </si>
+  <si>
+    <t>Erik</t>
+  </si>
+  <si>
+    <t>Wrolstad</t>
+  </si>
+  <si>
+    <t>Esther Bernstein</t>
+  </si>
+  <si>
+    <t>ebernstein</t>
+  </si>
+  <si>
+    <t>Esther</t>
+  </si>
+  <si>
+    <t>Bernstein</t>
+  </si>
+  <si>
+    <t>esther.bernstein@barclays.com</t>
+  </si>
+  <si>
+    <t>Jonathan Barufka</t>
+  </si>
+  <si>
+    <t>jbarufka</t>
+  </si>
+  <si>
+    <t>Jonathan</t>
+  </si>
+  <si>
+    <t>Barufka</t>
+  </si>
+  <si>
+    <t>jbarufka2</t>
+  </si>
+  <si>
+    <t>barufkajbcdf</t>
+  </si>
+  <si>
+    <t>barufkajbci</t>
+  </si>
+  <si>
+    <t>Jordan Tiger</t>
+  </si>
+  <si>
+    <t>jtiger</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Tiger</t>
+  </si>
+  <si>
+    <t>jordan.tiger@barclayscapital.com</t>
+  </si>
+  <si>
+    <t>Matias Bercun</t>
+  </si>
+  <si>
+    <t>mbercun</t>
+  </si>
+  <si>
+    <t>Matias</t>
+  </si>
+  <si>
+    <t>Bercun</t>
+  </si>
+  <si>
+    <t>Trader Trader</t>
+  </si>
+  <si>
+    <t>barcdevtrdv1</t>
+  </si>
+  <si>
+    <t>Trader</t>
+  </si>
+  <si>
+    <t>barcdevtrdv2</t>
+  </si>
+  <si>
+    <t>Xinji Gu</t>
+  </si>
+  <si>
+    <t>guxinjibcdf</t>
+  </si>
+  <si>
+    <t>Xinji</t>
+  </si>
+  <si>
+    <t>Gu</t>
+  </si>
+  <si>
+    <t>guxinjibci</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mm/dd/yyyy\ h:mm:ss\ AM/PM"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="5">
+    <numFmt numFmtId="167" formatCode="m/d/yy"/>
+    <numFmt numFmtId="168" formatCode="mmmm\ d\,\ yyyy"/>
+    <numFmt numFmtId="169" formatCode="0.00000000"/>
+    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="171" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -217,8 +502,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -231,8 +553,14 @@
         <bgColor theme="0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -255,29 +583,152 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="6" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="6" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -602,255 +1053,1451 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:K2"/>
+      <selection activeCell="F29" sqref="F29:F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="6" width="20.1640625" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="20.1640625" customWidth="1"/>
+    <col min="17" max="17" width="15.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9">
-      <c r="B2" s="7" t="s">
+    <row r="1" spans="2:17">
+      <c r="B1" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+    </row>
+    <row r="2" spans="2:17">
+      <c r="B2" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+    </row>
+    <row r="3" spans="2:17">
+      <c r="B3" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="24"/>
+    </row>
+    <row r="4" spans="2:17">
+      <c r="B4" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="22"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="10"/>
+    </row>
+    <row r="5" spans="2:17">
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="10"/>
+    </row>
+    <row r="6" spans="2:17" ht="26.25">
+      <c r="B6" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="M6" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="N6" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="O6" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="P6" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q6" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17">
+      <c r="B7" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" s="16">
+        <v>1</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J7" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="K7" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="L7" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="M7" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="N7" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="O7" s="18"/>
+      <c r="P7" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q7" s="21">
+        <v>42279.55889803241</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17">
+      <c r="B8" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8" s="16">
+        <v>1</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J8" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="K8" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="L8" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="M8" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="N8" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="O8" s="18"/>
+      <c r="P8" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q8" s="21">
+        <v>42275.583481400463</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17">
+      <c r="B9" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" s="16">
+        <v>1</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J9" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="K9" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="L9" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="M9" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="N9" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="O9" s="18"/>
+      <c r="P9" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q9" s="21">
+        <v>42286.582957905091</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17">
+      <c r="B10" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="G10" s="16">
+        <v>1</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J10" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="L10" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="M10" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="N10" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="O10" s="18"/>
+      <c r="P10" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q10" s="21">
+        <v>42284.694722604167</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17">
+      <c r="B11" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="G11" s="16">
+        <v>1</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J11" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="L11" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="M11" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="N11" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="O11" s="18"/>
+      <c r="P11" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q11" s="21">
+        <v>42034.951619988424</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17">
+      <c r="B12" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="G12" s="16"/>
+      <c r="H12" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="K12" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="L12" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="M12" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="N12" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="O12" s="18"/>
+      <c r="P12" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q12" s="21">
+        <v>41590.675543368059</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17">
+      <c r="B13" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="G13" s="16">
+        <v>1</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J13" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="K13" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="L13" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="M13" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="N13" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="O13" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="P13" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q13" s="21">
+        <v>42284.721531747688</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17">
+      <c r="B14" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="G14" s="16">
+        <v>1</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J14" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="K14" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="L14" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="M14" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="N14" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="O14" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="P14" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q14" s="21">
+        <v>42284.733527002318</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17">
+      <c r="B15" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="G15" s="16">
+        <v>1</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J15" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="K15" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="L15" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="M15" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="N15" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="O15" s="18"/>
+      <c r="P15" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q15" s="21">
+        <v>42017.610029479169</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17">
+      <c r="B16" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="G16" s="16"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J16" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="K16" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="L16" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="M16" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="N16" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="O16" s="18"/>
+      <c r="P16" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q16" s="21">
+        <v>42017.697332060183</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17">
+      <c r="B17" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G17" s="16"/>
+      <c r="H17" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="I17" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J17" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="K17" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="L17" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="M17" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="N17" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="O17" s="18"/>
+      <c r="P17" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q17" s="21">
+        <v>41585.85667523148</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17">
+      <c r="B18" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="G18" s="16">
+        <v>1</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="I18" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J18" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="K18" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="L18" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="M18" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="N18" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="O18" s="18"/>
+      <c r="P18" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q18" s="21">
+        <v>42278.593576388892</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17">
+      <c r="B19" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="G19" s="16">
+        <v>1</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J19" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="K19" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="L19" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="M19" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="N19" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="O19" s="18"/>
+      <c r="P19" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q19" s="21">
+        <v>42282.628477928243</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17">
+      <c r="B20" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="G20" s="16">
+        <v>1</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J20" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="K20" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="L20" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="M20" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="N20" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="O20" s="18"/>
+      <c r="P20" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q20" s="21">
+        <v>42291.560386111109</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17">
+      <c r="B21" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="G21" s="16">
+        <v>1</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="I21" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J21" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="K21" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="L21" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="M21" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="N21" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="O21" s="18"/>
+      <c r="P21" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q21" s="21">
+        <v>42286.714989120374</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17">
+      <c r="B22" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="G22" s="16"/>
+      <c r="H22" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="I22" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J22" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="K22" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="L22" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="M22" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="N22" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="O22" s="18"/>
+      <c r="P22" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q22" s="21">
+        <v>41676.777017858796</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17">
+      <c r="B23" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="G23" s="16"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J23" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="K23" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="L23" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="M23" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="N23" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="O23" s="18"/>
+      <c r="P23" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q23" s="21">
+        <v>41218.541249270835</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17">
+      <c r="B24" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="G24" s="16">
+        <v>1</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J24" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="K24" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="L24" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="M24" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="N24" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="O24" s="18"/>
+      <c r="P24" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q24" s="21">
+        <v>42279.598463194445</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17">
+      <c r="B25" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="G25" s="16">
+        <v>1</v>
+      </c>
+      <c r="H25" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="I25" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J25" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="K25" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="L25" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="M25" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="N25" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="O25" s="18"/>
+      <c r="P25" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q25" s="21">
+        <v>42262.840839814817</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17">
+      <c r="B26" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="G26" s="16">
+        <v>1</v>
+      </c>
+      <c r="H26" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="I26" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J26" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="K26" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="L26" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="M26" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="N26" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="O26" s="18"/>
+      <c r="P26" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q26" s="21">
+        <v>42290.711832719906</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17">
+      <c r="B27" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="G27" s="16">
+        <v>1</v>
+      </c>
+      <c r="H27" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="I27" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J27" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="K27" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="L27" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="M27" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="N27" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="O27" s="18"/>
+      <c r="P27" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q27" s="21">
+        <v>42290.834409722222</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B1:Q1"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="B3:Q3"/>
+    <mergeCell ref="F4:I4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C2:J23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19:C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="3" max="7" width="20.125" customWidth="1"/>
+    <col min="8" max="8" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="20.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:10">
+      <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-    </row>
-    <row r="3" spans="2:9">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-    </row>
-    <row r="6" spans="2:9" s="1" customFormat="1">
-      <c r="B6" s="2" t="s">
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+    </row>
+    <row r="3" spans="3:10">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+    </row>
+    <row r="6" spans="3:10" s="1" customFormat="1">
+      <c r="C6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:9">
-      <c r="B7" s="3" t="s">
+    <row r="7" spans="3:10">
+      <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="F7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="G7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="5">
-        <v>42016.664583333331</v>
-      </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
-      <c r="B8" s="3" t="s">
+    <row r="8" spans="3:10">
+      <c r="C8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="E8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="G8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="5">
-        <v>42017.664583275466</v>
-      </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="J8" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="2:9">
-      <c r="B9" s="3" t="s">
+    <row r="9" spans="3:10">
+      <c r="C9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="F9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="G9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="5">
-        <v>42018.664583275466</v>
-      </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="J9" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:9">
-      <c r="B10" s="3" t="s">
+    <row r="10" spans="3:10">
+      <c r="C10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="E10" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="F10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="G10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="5">
-        <v>42019.664583275466</v>
-      </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="J10" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="2:9">
-      <c r="B11" s="3" t="s">
+    <row r="11" spans="3:10">
+      <c r="C11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="F11" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="G11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="5">
-        <v>42020.664583275466</v>
-      </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="J11" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="2:9">
-      <c r="B12" s="3" t="s">
+    <row r="12" spans="3:10">
+      <c r="C12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="E12" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="F12" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="G12" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="5">
-        <v>42021.664583275466</v>
-      </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="J12" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="2:9">
-      <c r="B13" s="3" t="s">
+    <row r="13" spans="3:10">
+      <c r="C13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="E13" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="F13" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="G13" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="5">
-        <v>42022.664583275466</v>
-      </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="I13" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="J13" s="3" t="s">
         <v>57</v>
       </c>
+    </row>
+    <row r="16" spans="3:10">
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="8:8">
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="8:8">
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="8:8">
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="8:8">
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="8:8">
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="8:8">
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="8:8">
+      <c r="H23" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="C3:J3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>